<commit_message>
Added documentation and staging runbook
</commit_message>
<xml_diff>
--- a/RPi Pinout_Test_Board.xlsx
+++ b/RPi Pinout_Test_Board.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davist/Documents/Events/Events 2018/vForum 2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davist/vforum2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E06054-E255-AC49-A4E7-5C793899CBFF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D102DF-8FFB-E243-8865-F20DF0D1BE82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="460" windowWidth="23180" windowHeight="14120" activeTab="1" xr2:uid="{085A2C76-9AE2-8C42-9C80-B71D799E845C}"/>
+    <workbookView xWindow="3360" yWindow="460" windowWidth="18880" windowHeight="14140" xr2:uid="{085A2C76-9AE2-8C42-9C80-B71D799E845C}"/>
   </bookViews>
   <sheets>
-    <sheet name="4WD" sheetId="1" r:id="rId1"/>
-    <sheet name="Tank" sheetId="2" r:id="rId2"/>
+    <sheet name="Tank" sheetId="2" r:id="rId1"/>
+    <sheet name="4WD" sheetId="1" r:id="rId2"/>
     <sheet name="PAN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Pin</t>
   </si>
@@ -117,14 +117,43 @@
   </si>
   <si>
     <t>lft_mtr_enable</t>
+  </si>
+  <si>
+    <t>rt_ena</t>
+  </si>
+  <si>
+    <t>lft_ena</t>
+  </si>
+  <si>
+    <t>BCM</t>
+  </si>
+  <si>
+    <t>BOARD</t>
+  </si>
+  <si>
+    <t>PIN NUMBER</t>
+  </si>
+  <si>
+    <t>GPIO #</t>
+  </si>
+  <si>
+    <t>PIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -152,8 +181,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,6 +214,116 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>190102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB2DB82-5E4E-F94C-8EF3-D79EE7E11E4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1358900" y="8420099"/>
+          <a:ext cx="2019300" cy="6121003"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12699</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>205434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="http://pi4j.com/images/j8header-3b.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B7A480-190E-8147-9C03-11E75FF26B0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3251200" y="445084"/>
+          <a:ext cx="3746499" cy="6796150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -259,116 +411,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="10299700" y="1739900"/>
-          <a:ext cx="6350000" cy="11518900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>101202</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB2DB82-5E4E-F94C-8EF3-D79EE7E11E4D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3517900" y="101599"/>
-          <a:ext cx="2019300" cy="6121003"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1409700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="http://pi4j.com/images/j8header-3b.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B7A480-190E-8147-9C03-11E75FF26B0E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7505700" y="0"/>
           <a:ext cx="6350000" cy="11518900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -841,6 +883,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F04E73-0081-464D-8922-96A2EB285FDD}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BDE006-33D6-E349-8DEB-0098A35487A9}">
   <dimension ref="B2:H28"/>
   <sheetViews>
@@ -996,173 +1218,6 @@
     <row r="26" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F04E73-0081-464D-8922-96A2EB285FDD}">
-  <dimension ref="A2:H28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="7" max="7" width="4.83203125" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G11">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G13">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18">
-        <v>32</v>
-      </c>
-      <c r="H18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G20">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G21">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G22">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>